<commit_message>
solved excell width problem
</commit_message>
<xml_diff>
--- a/semester2.xlsx
+++ b/semester2.xlsx
@@ -432,6 +432,11 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="26" customWidth="1" min="1" max="1"/>
+    <col width="14" customWidth="1" min="2" max="2"/>
+    <col width="6" customWidth="1" min="3" max="3"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -458,13 +463,11 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>. GT24BCAR001</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>8.52</t>
-        </is>
+          <t xml:space="preserve"> GT24BCAR001</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>8.52</v>
       </c>
     </row>
     <row r="3">
@@ -475,13 +478,11 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>. GT24BCAR002</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>6.43</t>
-        </is>
+          <t xml:space="preserve"> GT24BCAR002</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>6.43</v>
       </c>
     </row>
     <row r="4">
@@ -492,13 +493,11 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>. GT24BCAR003</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>--</t>
-        </is>
+          <t xml:space="preserve"> GT24BCAR003</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -509,13 +508,11 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>. GT24BCAR006</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>8.10</t>
-        </is>
+          <t xml:space="preserve"> GT24BCAR006</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>8.1</v>
       </c>
     </row>
     <row r="6">
@@ -526,13 +523,11 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>. GT24BCAR007</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>6.90</t>
-        </is>
+          <t xml:space="preserve"> GT24BCAR007</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>6.9</v>
       </c>
     </row>
     <row r="7">
@@ -543,13 +538,11 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>. GT24BCAR008</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>--</t>
-        </is>
+          <t xml:space="preserve"> GT24BCAR008</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -560,13 +553,11 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>. GT24BCAR009</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>7.71</t>
-        </is>
+          <t xml:space="preserve"> GT24BCAR009</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>7.71</v>
       </c>
     </row>
     <row r="9">
@@ -577,13 +568,11 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>. GT24BCAR011</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>7.00</t>
-        </is>
+          <t xml:space="preserve"> GT24BCAR011</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="10">
@@ -594,13 +583,11 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>. GT24BCAR013</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>6.19</t>
-        </is>
+          <t xml:space="preserve"> GT24BCAR013</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>6.19</v>
       </c>
     </row>
     <row r="11">
@@ -611,13 +598,11 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>. GT24BCAR014</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>--</t>
-        </is>
+          <t xml:space="preserve"> GT24BCAR014</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -628,13 +613,11 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>. GT24BCAR015</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>8.05</t>
-        </is>
+          <t xml:space="preserve"> GT24BCAR015</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>8.050000000000001</v>
       </c>
     </row>
     <row r="13">
@@ -645,13 +628,11 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>. GT24BCAR016</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>6.76</t>
-        </is>
+          <t xml:space="preserve"> GT24BCAR016</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>6.76</v>
       </c>
     </row>
     <row r="14">
@@ -662,13 +643,11 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>. GT24BCAR017</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>7.95</t>
-        </is>
+          <t xml:space="preserve"> GT24BCAR017</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>7.95</v>
       </c>
     </row>
     <row r="15">
@@ -679,13 +658,11 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>. GT24BCAR018</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>7.19</t>
-        </is>
+          <t xml:space="preserve"> GT24BCAR018</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>7.19</v>
       </c>
     </row>
     <row r="16">
@@ -696,13 +673,11 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>. GT24BCAR019</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>7.95</t>
-        </is>
+          <t xml:space="preserve"> GT24BCAR019</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>7.95</v>
       </c>
     </row>
     <row r="17">
@@ -713,13 +688,11 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>. GT24BCAR020</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>8.24</t>
-        </is>
+          <t xml:space="preserve"> GT24BCAR020</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>8.24</v>
       </c>
     </row>
     <row r="18">
@@ -730,13 +703,11 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>. GT24BCAR021</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>6.57</t>
-        </is>
+          <t xml:space="preserve"> GT24BCAR021</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>6.57</v>
       </c>
     </row>
     <row r="19">
@@ -747,13 +718,11 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>. GT24BCAR023</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>6.33</t>
-        </is>
+          <t xml:space="preserve"> GT24BCAR023</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>6.33</v>
       </c>
     </row>
     <row r="20">
@@ -764,13 +733,11 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>. GT24BCAR024</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>6.90</t>
-        </is>
+          <t xml:space="preserve"> GT24BCAR024</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>6.9</v>
       </c>
     </row>
     <row r="21">
@@ -781,13 +748,11 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>. GT24BCAR025</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>--</t>
-        </is>
+          <t xml:space="preserve"> GT24BCAR025</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -798,13 +763,11 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>. GT24BCAR026</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>6.90</t>
-        </is>
+          <t xml:space="preserve"> GT24BCAR026</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>6.9</v>
       </c>
     </row>
     <row r="23">
@@ -815,13 +778,11 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>. GT24BCAR027</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>7.71</t>
-        </is>
+          <t xml:space="preserve"> GT24BCAR027</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>7.71</v>
       </c>
     </row>
     <row r="24">
@@ -832,13 +793,11 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>. GT24BCAR028</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>8.62</t>
-        </is>
+          <t xml:space="preserve"> GT24BCAR028</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>8.619999999999999</v>
       </c>
     </row>
     <row r="25">
@@ -849,13 +808,11 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>. GT24BCAR029</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>6.14</t>
-        </is>
+          <t xml:space="preserve"> GT24BCAR029</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>6.14</v>
       </c>
     </row>
     <row r="26">
@@ -866,13 +823,11 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>. GT24BCAR030</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>--</t>
-        </is>
+          <t xml:space="preserve"> GT24BCAR030</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -883,13 +838,11 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>. GT24BCAR031</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>6.05</t>
-        </is>
+          <t xml:space="preserve"> GT24BCAR031</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>6.05</v>
       </c>
     </row>
     <row r="28">
@@ -900,13 +853,11 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>. GT24BCAR032</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>7.19</t>
-        </is>
+          <t xml:space="preserve"> GT24BCAR032</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>7.19</v>
       </c>
     </row>
     <row r="29">
@@ -917,13 +868,11 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>. GT24BCAR034</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>7.00</t>
-        </is>
+          <t xml:space="preserve"> GT24BCAR034</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="30">
@@ -934,13 +883,11 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>. GT24BCAR004</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>7.24</t>
-        </is>
+          <t xml:space="preserve"> GT24BCAR004</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>7.24</v>
       </c>
     </row>
     <row r="31">
@@ -951,13 +898,11 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>. GT24BCAR022</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>6.76</t>
-        </is>
+          <t xml:space="preserve"> GT24BCAR022</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>6.76</v>
       </c>
     </row>
     <row r="32">
@@ -968,13 +913,11 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>. GT24BCAR033</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>7.33</t>
-        </is>
+          <t xml:space="preserve"> GT24BCAR033</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>7.33</v>
       </c>
     </row>
     <row r="33">
@@ -985,13 +928,11 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>. GT24BCAR035</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>8.52</t>
-        </is>
+          <t xml:space="preserve"> GT24BCAR035</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>8.52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
an error came by "ValueError: All arrays must be of the same length"
</commit_message>
<xml_diff>
--- a/semester2.xlsx
+++ b/semester2.xlsx
@@ -425,18 +425,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:D129"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="26" customWidth="1" min="1" max="1"/>
-    <col width="14" customWidth="1" min="2" max="2"/>
-    <col width="6" customWidth="1" min="3" max="3"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -451,6 +446,11 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>AEC</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>SGPA</t>
         </is>
       </c>
@@ -466,7 +466,12 @@
           <t xml:space="preserve"> GT24BCAR001</t>
         </is>
       </c>
-      <c r="C2" t="n">
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
         <v>8.52</v>
       </c>
     </row>
@@ -481,7 +486,12 @@
           <t xml:space="preserve"> GT24BCAR002</t>
         </is>
       </c>
-      <c r="C3" t="n">
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
         <v>6.43</v>
       </c>
     </row>
@@ -496,7 +506,12 @@
           <t xml:space="preserve"> GT24BCAR003</t>
         </is>
       </c>
-      <c r="C4" t="n">
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -511,7 +526,12 @@
           <t xml:space="preserve"> GT24BCAR006</t>
         </is>
       </c>
-      <c r="C5" t="n">
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
         <v>8.1</v>
       </c>
     </row>
@@ -526,7 +546,12 @@
           <t xml:space="preserve"> GT24BCAR007</t>
         </is>
       </c>
-      <c r="C6" t="n">
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
         <v>6.9</v>
       </c>
     </row>
@@ -541,7 +566,12 @@
           <t xml:space="preserve"> GT24BCAR008</t>
         </is>
       </c>
-      <c r="C7" t="n">
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -556,7 +586,12 @@
           <t xml:space="preserve"> GT24BCAR009</t>
         </is>
       </c>
-      <c r="C8" t="n">
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
         <v>7.71</v>
       </c>
     </row>
@@ -571,7 +606,12 @@
           <t xml:space="preserve"> GT24BCAR011</t>
         </is>
       </c>
-      <c r="C9" t="n">
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
         <v>7</v>
       </c>
     </row>
@@ -586,7 +626,12 @@
           <t xml:space="preserve"> GT24BCAR013</t>
         </is>
       </c>
-      <c r="C10" t="n">
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
         <v>6.19</v>
       </c>
     </row>
@@ -601,7 +646,12 @@
           <t xml:space="preserve"> GT24BCAR014</t>
         </is>
       </c>
-      <c r="C11" t="n">
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
         <v>0</v>
       </c>
     </row>
@@ -616,7 +666,12 @@
           <t xml:space="preserve"> GT24BCAR015</t>
         </is>
       </c>
-      <c r="C12" t="n">
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
         <v>8.050000000000001</v>
       </c>
     </row>
@@ -631,7 +686,12 @@
           <t xml:space="preserve"> GT24BCAR016</t>
         </is>
       </c>
-      <c r="C13" t="n">
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
         <v>6.76</v>
       </c>
     </row>
@@ -646,7 +706,12 @@
           <t xml:space="preserve"> GT24BCAR017</t>
         </is>
       </c>
-      <c r="C14" t="n">
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
         <v>7.95</v>
       </c>
     </row>
@@ -661,7 +726,12 @@
           <t xml:space="preserve"> GT24BCAR018</t>
         </is>
       </c>
-      <c r="C15" t="n">
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
         <v>7.19</v>
       </c>
     </row>
@@ -676,7 +746,12 @@
           <t xml:space="preserve"> GT24BCAR019</t>
         </is>
       </c>
-      <c r="C16" t="n">
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
         <v>7.95</v>
       </c>
     </row>
@@ -691,7 +766,12 @@
           <t xml:space="preserve"> GT24BCAR020</t>
         </is>
       </c>
-      <c r="C17" t="n">
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
         <v>8.24</v>
       </c>
     </row>
@@ -706,7 +786,12 @@
           <t xml:space="preserve"> GT24BCAR021</t>
         </is>
       </c>
-      <c r="C18" t="n">
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
         <v>6.57</v>
       </c>
     </row>
@@ -721,7 +806,12 @@
           <t xml:space="preserve"> GT24BCAR023</t>
         </is>
       </c>
-      <c r="C19" t="n">
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
         <v>6.33</v>
       </c>
     </row>
@@ -736,7 +826,12 @@
           <t xml:space="preserve"> GT24BCAR024</t>
         </is>
       </c>
-      <c r="C20" t="n">
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
         <v>6.9</v>
       </c>
     </row>
@@ -751,7 +846,12 @@
           <t xml:space="preserve"> GT24BCAR025</t>
         </is>
       </c>
-      <c r="C21" t="n">
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
         <v>0</v>
       </c>
     </row>
@@ -766,7 +866,12 @@
           <t xml:space="preserve"> GT24BCAR026</t>
         </is>
       </c>
-      <c r="C22" t="n">
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
         <v>6.9</v>
       </c>
     </row>
@@ -781,7 +886,12 @@
           <t xml:space="preserve"> GT24BCAR027</t>
         </is>
       </c>
-      <c r="C23" t="n">
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
         <v>7.71</v>
       </c>
     </row>
@@ -796,7 +906,12 @@
           <t xml:space="preserve"> GT24BCAR028</t>
         </is>
       </c>
-      <c r="C24" t="n">
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
         <v>8.619999999999999</v>
       </c>
     </row>
@@ -811,7 +926,12 @@
           <t xml:space="preserve"> GT24BCAR029</t>
         </is>
       </c>
-      <c r="C25" t="n">
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
         <v>6.14</v>
       </c>
     </row>
@@ -826,7 +946,12 @@
           <t xml:space="preserve"> GT24BCAR030</t>
         </is>
       </c>
-      <c r="C26" t="n">
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
         <v>0</v>
       </c>
     </row>
@@ -841,7 +966,12 @@
           <t xml:space="preserve"> GT24BCAR031</t>
         </is>
       </c>
-      <c r="C27" t="n">
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
         <v>6.05</v>
       </c>
     </row>
@@ -856,7 +986,12 @@
           <t xml:space="preserve"> GT24BCAR032</t>
         </is>
       </c>
-      <c r="C28" t="n">
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
         <v>7.19</v>
       </c>
     </row>
@@ -871,7 +1006,12 @@
           <t xml:space="preserve"> GT24BCAR034</t>
         </is>
       </c>
-      <c r="C29" t="n">
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
         <v>7</v>
       </c>
     </row>
@@ -886,7 +1026,12 @@
           <t xml:space="preserve"> GT24BCAR004</t>
         </is>
       </c>
-      <c r="C30" t="n">
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
         <v>7.24</v>
       </c>
     </row>
@@ -901,7 +1046,12 @@
           <t xml:space="preserve"> GT24BCAR022</t>
         </is>
       </c>
-      <c r="C31" t="n">
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
         <v>6.76</v>
       </c>
     </row>
@@ -916,7 +1066,12 @@
           <t xml:space="preserve"> GT24BCAR033</t>
         </is>
       </c>
-      <c r="C32" t="n">
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
         <v>7.33</v>
       </c>
     </row>
@@ -931,7 +1086,1740 @@
           <t xml:space="preserve"> GT24BCAR035</t>
         </is>
       </c>
-      <c r="C33" t="n">
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>8.52</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>DIYA AZGAR</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR001</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>9</v>
+      </c>
+      <c r="D34" t="n">
+        <v>8.52</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>MUHAMMED SAJAD .N</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR002</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>7</v>
+      </c>
+      <c r="D35" t="n">
+        <v>6.43</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>ADWAYA SHAJI</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR003</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>8</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>ABHINAV K K</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR006</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>8</v>
+      </c>
+      <c r="D37" t="n">
+        <v>8.1</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>ABHINAV P</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR007</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>8</v>
+      </c>
+      <c r="D38" t="n">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>ABHISHEK SURENDRAN</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR008</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>8</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>ADITHYADEV K</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR009</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>8</v>
+      </c>
+      <c r="D40" t="n">
+        <v>7.71</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>AMAL ARAVIND.K</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR011</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>7</v>
+      </c>
+      <c r="D41" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>VIGHNEY A</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR013</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>8</v>
+      </c>
+      <c r="D42" t="n">
+        <v>6.19</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>YADHUL A</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR014</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>7</v>
+      </c>
+      <c r="D43" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>ATHEETHA K</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR015</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>8</v>
+      </c>
+      <c r="D44" t="n">
+        <v>8.050000000000001</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>DEVANANDA DILEEP</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR016</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>7</v>
+      </c>
+      <c r="D45" t="n">
+        <v>6.76</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>HRISHAYA K</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR017</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>8</v>
+      </c>
+      <c r="D46" t="n">
+        <v>7.95</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>PARVANA AJITH</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR018</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>8</v>
+      </c>
+      <c r="D47" t="n">
+        <v>7.19</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>SANIYA BABU M P</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR019</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>8</v>
+      </c>
+      <c r="D48" t="n">
+        <v>7.95</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>SREEPRIYA N</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR020</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>8</v>
+      </c>
+      <c r="D49" t="n">
+        <v>8.24</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>THANISHKA .D</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR021</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>7</v>
+      </c>
+      <c r="D50" t="n">
+        <v>6.57</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>ABHINAND.V</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR023</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
+        <v>8</v>
+      </c>
+      <c r="D51" t="n">
+        <v>6.33</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>ADWAID K</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR024</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>8</v>
+      </c>
+      <c r="D52" t="n">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>AKSHAI KUMAR P P</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR025</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>7</v>
+      </c>
+      <c r="D53" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>ANURANJ E</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR026</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>8</v>
+      </c>
+      <c r="D54" t="n">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>DHYAN DILEEP</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR027</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>8</v>
+      </c>
+      <c r="D55" t="n">
+        <v>7.71</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>ESHAN SHAH K</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR028</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>8</v>
+      </c>
+      <c r="D56" t="n">
+        <v>8.619999999999999</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>GOUTHAM SANKAR PUTHUKUDI</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR029</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>8</v>
+      </c>
+      <c r="D57" t="n">
+        <v>6.14</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>MUHAMMED ASHIR P.P</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR030</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>6</v>
+      </c>
+      <c r="D58" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>SAYANTH T M</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR031</t>
+        </is>
+      </c>
+      <c r="C59" t="n">
+        <v>7</v>
+      </c>
+      <c r="D59" t="n">
+        <v>6.05</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>SAYOOJ A K</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR032</t>
+        </is>
+      </c>
+      <c r="C60" t="n">
+        <v>8</v>
+      </c>
+      <c r="D60" t="n">
+        <v>7.19</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>SREENANDH. A. P</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR034</t>
+        </is>
+      </c>
+      <c r="C61" t="n">
+        <v>7</v>
+      </c>
+      <c r="D61" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>SANDAL FARIYA</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR004</t>
+        </is>
+      </c>
+      <c r="C62" t="n">
+        <v>8</v>
+      </c>
+      <c r="D62" t="n">
+        <v>7.24</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>ABHIJITH K</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR022</t>
+        </is>
+      </c>
+      <c r="C63" t="n">
+        <v>7</v>
+      </c>
+      <c r="D63" t="n">
+        <v>6.76</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>SHALVIN P</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR033</t>
+        </is>
+      </c>
+      <c r="C64" t="n">
+        <v>7</v>
+      </c>
+      <c r="D64" t="n">
+        <v>7.33</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>SRIDHUN .P</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR035</t>
+        </is>
+      </c>
+      <c r="C65" t="n">
+        <v>8</v>
+      </c>
+      <c r="D65" t="n">
+        <v>8.52</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>DIYA AZGAR</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR001</t>
+        </is>
+      </c>
+      <c r="C66" t="n">
+        <v>9</v>
+      </c>
+      <c r="D66" t="n">
+        <v>8.52</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>MUHAMMED SAJAD .N</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR002</t>
+        </is>
+      </c>
+      <c r="C67" t="n">
+        <v>7</v>
+      </c>
+      <c r="D67" t="n">
+        <v>6.43</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>ADWAYA SHAJI</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR003</t>
+        </is>
+      </c>
+      <c r="C68" t="n">
+        <v>8</v>
+      </c>
+      <c r="D68" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>ABHINAV K K</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR006</t>
+        </is>
+      </c>
+      <c r="C69" t="n">
+        <v>8</v>
+      </c>
+      <c r="D69" t="n">
+        <v>8.1</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>ABHINAV P</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR007</t>
+        </is>
+      </c>
+      <c r="C70" t="n">
+        <v>8</v>
+      </c>
+      <c r="D70" t="n">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>ABHISHEK SURENDRAN</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR008</t>
+        </is>
+      </c>
+      <c r="C71" t="n">
+        <v>8</v>
+      </c>
+      <c r="D71" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>ADITHYADEV K</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR009</t>
+        </is>
+      </c>
+      <c r="C72" t="n">
+        <v>8</v>
+      </c>
+      <c r="D72" t="n">
+        <v>7.71</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>AMAL ARAVIND.K</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR011</t>
+        </is>
+      </c>
+      <c r="C73" t="n">
+        <v>7</v>
+      </c>
+      <c r="D73" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>VIGHNEY A</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR013</t>
+        </is>
+      </c>
+      <c r="C74" t="n">
+        <v>8</v>
+      </c>
+      <c r="D74" t="n">
+        <v>6.19</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>YADHUL A</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR014</t>
+        </is>
+      </c>
+      <c r="C75" t="n">
+        <v>7</v>
+      </c>
+      <c r="D75" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>ATHEETHA K</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR015</t>
+        </is>
+      </c>
+      <c r="C76" t="n">
+        <v>8</v>
+      </c>
+      <c r="D76" t="n">
+        <v>8.050000000000001</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>DEVANANDA DILEEP</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR016</t>
+        </is>
+      </c>
+      <c r="C77" t="n">
+        <v>7</v>
+      </c>
+      <c r="D77" t="n">
+        <v>6.76</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>HRISHAYA K</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR017</t>
+        </is>
+      </c>
+      <c r="C78" t="n">
+        <v>8</v>
+      </c>
+      <c r="D78" t="n">
+        <v>7.95</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>PARVANA AJITH</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR018</t>
+        </is>
+      </c>
+      <c r="C79" t="n">
+        <v>8</v>
+      </c>
+      <c r="D79" t="n">
+        <v>7.19</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>SANIYA BABU M P</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR019</t>
+        </is>
+      </c>
+      <c r="C80" t="n">
+        <v>8</v>
+      </c>
+      <c r="D80" t="n">
+        <v>7.95</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>SREEPRIYA N</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR020</t>
+        </is>
+      </c>
+      <c r="C81" t="n">
+        <v>8</v>
+      </c>
+      <c r="D81" t="n">
+        <v>8.24</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>THANISHKA .D</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR021</t>
+        </is>
+      </c>
+      <c r="C82" t="n">
+        <v>7</v>
+      </c>
+      <c r="D82" t="n">
+        <v>6.57</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>ABHINAND.V</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR023</t>
+        </is>
+      </c>
+      <c r="C83" t="n">
+        <v>8</v>
+      </c>
+      <c r="D83" t="n">
+        <v>6.33</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>ADWAID K</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR024</t>
+        </is>
+      </c>
+      <c r="C84" t="n">
+        <v>8</v>
+      </c>
+      <c r="D84" t="n">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>AKSHAI KUMAR P P</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR025</t>
+        </is>
+      </c>
+      <c r="C85" t="n">
+        <v>7</v>
+      </c>
+      <c r="D85" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>ANURANJ E</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR026</t>
+        </is>
+      </c>
+      <c r="C86" t="n">
+        <v>8</v>
+      </c>
+      <c r="D86" t="n">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>DHYAN DILEEP</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR027</t>
+        </is>
+      </c>
+      <c r="C87" t="n">
+        <v>8</v>
+      </c>
+      <c r="D87" t="n">
+        <v>7.71</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>ESHAN SHAH K</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR028</t>
+        </is>
+      </c>
+      <c r="C88" t="n">
+        <v>8</v>
+      </c>
+      <c r="D88" t="n">
+        <v>8.619999999999999</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>GOUTHAM SANKAR PUTHUKUDI</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR029</t>
+        </is>
+      </c>
+      <c r="C89" t="n">
+        <v>8</v>
+      </c>
+      <c r="D89" t="n">
+        <v>6.14</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>MUHAMMED ASHIR P.P</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR030</t>
+        </is>
+      </c>
+      <c r="C90" t="n">
+        <v>6</v>
+      </c>
+      <c r="D90" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>SAYANTH T M</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR031</t>
+        </is>
+      </c>
+      <c r="C91" t="n">
+        <v>7</v>
+      </c>
+      <c r="D91" t="n">
+        <v>6.05</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>SAYOOJ A K</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR032</t>
+        </is>
+      </c>
+      <c r="C92" t="n">
+        <v>8</v>
+      </c>
+      <c r="D92" t="n">
+        <v>7.19</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>SREENANDH. A. P</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR034</t>
+        </is>
+      </c>
+      <c r="C93" t="n">
+        <v>7</v>
+      </c>
+      <c r="D93" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>SANDAL FARIYA</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR004</t>
+        </is>
+      </c>
+      <c r="C94" t="n">
+        <v>8</v>
+      </c>
+      <c r="D94" t="n">
+        <v>7.24</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>ABHIJITH K</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR022</t>
+        </is>
+      </c>
+      <c r="C95" t="n">
+        <v>7</v>
+      </c>
+      <c r="D95" t="n">
+        <v>6.76</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>SHALVIN P</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR033</t>
+        </is>
+      </c>
+      <c r="C96" t="n">
+        <v>7</v>
+      </c>
+      <c r="D96" t="n">
+        <v>7.33</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>SRIDHUN .P</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR035</t>
+        </is>
+      </c>
+      <c r="C97" t="n">
+        <v>8</v>
+      </c>
+      <c r="D97" t="n">
+        <v>8.52</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>DIYA AZGAR</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR001</t>
+        </is>
+      </c>
+      <c r="C98" t="n">
+        <v>9</v>
+      </c>
+      <c r="D98" t="n">
+        <v>8.52</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>MUHAMMED SAJAD .N</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR002</t>
+        </is>
+      </c>
+      <c r="C99" t="n">
+        <v>7</v>
+      </c>
+      <c r="D99" t="n">
+        <v>6.43</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>ADWAYA SHAJI</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR003</t>
+        </is>
+      </c>
+      <c r="C100" t="n">
+        <v>8</v>
+      </c>
+      <c r="D100" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>ABHINAV K K</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR006</t>
+        </is>
+      </c>
+      <c r="C101" t="n">
+        <v>8</v>
+      </c>
+      <c r="D101" t="n">
+        <v>8.1</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>ABHINAV P</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR007</t>
+        </is>
+      </c>
+      <c r="C102" t="n">
+        <v>8</v>
+      </c>
+      <c r="D102" t="n">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>ABHISHEK SURENDRAN</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR008</t>
+        </is>
+      </c>
+      <c r="C103" t="n">
+        <v>8</v>
+      </c>
+      <c r="D103" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>ADITHYADEV K</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR009</t>
+        </is>
+      </c>
+      <c r="C104" t="n">
+        <v>8</v>
+      </c>
+      <c r="D104" t="n">
+        <v>7.71</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>AMAL ARAVIND.K</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR011</t>
+        </is>
+      </c>
+      <c r="C105" t="n">
+        <v>7</v>
+      </c>
+      <c r="D105" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>VIGHNEY A</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR013</t>
+        </is>
+      </c>
+      <c r="C106" t="n">
+        <v>8</v>
+      </c>
+      <c r="D106" t="n">
+        <v>6.19</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>YADHUL A</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR014</t>
+        </is>
+      </c>
+      <c r="C107" t="n">
+        <v>7</v>
+      </c>
+      <c r="D107" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>ATHEETHA K</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR015</t>
+        </is>
+      </c>
+      <c r="C108" t="n">
+        <v>8</v>
+      </c>
+      <c r="D108" t="n">
+        <v>8.050000000000001</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>DEVANANDA DILEEP</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR016</t>
+        </is>
+      </c>
+      <c r="C109" t="n">
+        <v>7</v>
+      </c>
+      <c r="D109" t="n">
+        <v>6.76</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>HRISHAYA K</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR017</t>
+        </is>
+      </c>
+      <c r="C110" t="n">
+        <v>8</v>
+      </c>
+      <c r="D110" t="n">
+        <v>7.95</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>PARVANA AJITH</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR018</t>
+        </is>
+      </c>
+      <c r="C111" t="n">
+        <v>8</v>
+      </c>
+      <c r="D111" t="n">
+        <v>7.19</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>SANIYA BABU M P</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR019</t>
+        </is>
+      </c>
+      <c r="C112" t="n">
+        <v>8</v>
+      </c>
+      <c r="D112" t="n">
+        <v>7.95</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>SREEPRIYA N</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR020</t>
+        </is>
+      </c>
+      <c r="C113" t="n">
+        <v>8</v>
+      </c>
+      <c r="D113" t="n">
+        <v>8.24</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>THANISHKA .D</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR021</t>
+        </is>
+      </c>
+      <c r="C114" t="n">
+        <v>7</v>
+      </c>
+      <c r="D114" t="n">
+        <v>6.57</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>ABHINAND.V</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR023</t>
+        </is>
+      </c>
+      <c r="C115" t="n">
+        <v>8</v>
+      </c>
+      <c r="D115" t="n">
+        <v>6.33</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>ADWAID K</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR024</t>
+        </is>
+      </c>
+      <c r="C116" t="n">
+        <v>8</v>
+      </c>
+      <c r="D116" t="n">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>AKSHAI KUMAR P P</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR025</t>
+        </is>
+      </c>
+      <c r="C117" t="n">
+        <v>7</v>
+      </c>
+      <c r="D117" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>ANURANJ E</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR026</t>
+        </is>
+      </c>
+      <c r="C118" t="n">
+        <v>8</v>
+      </c>
+      <c r="D118" t="n">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>DHYAN DILEEP</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR027</t>
+        </is>
+      </c>
+      <c r="C119" t="n">
+        <v>8</v>
+      </c>
+      <c r="D119" t="n">
+        <v>7.71</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>ESHAN SHAH K</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR028</t>
+        </is>
+      </c>
+      <c r="C120" t="n">
+        <v>8</v>
+      </c>
+      <c r="D120" t="n">
+        <v>8.619999999999999</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>GOUTHAM SANKAR PUTHUKUDI</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR029</t>
+        </is>
+      </c>
+      <c r="C121" t="n">
+        <v>8</v>
+      </c>
+      <c r="D121" t="n">
+        <v>6.14</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>MUHAMMED ASHIR P.P</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR030</t>
+        </is>
+      </c>
+      <c r="C122" t="n">
+        <v>6</v>
+      </c>
+      <c r="D122" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>SAYANTH T M</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR031</t>
+        </is>
+      </c>
+      <c r="C123" t="n">
+        <v>7</v>
+      </c>
+      <c r="D123" t="n">
+        <v>6.05</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>SAYOOJ A K</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR032</t>
+        </is>
+      </c>
+      <c r="C124" t="n">
+        <v>8</v>
+      </c>
+      <c r="D124" t="n">
+        <v>7.19</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>SREENANDH. A. P</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR034</t>
+        </is>
+      </c>
+      <c r="C125" t="n">
+        <v>7</v>
+      </c>
+      <c r="D125" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>SANDAL FARIYA</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR004</t>
+        </is>
+      </c>
+      <c r="C126" t="n">
+        <v>8</v>
+      </c>
+      <c r="D126" t="n">
+        <v>7.24</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>ABHIJITH K</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR022</t>
+        </is>
+      </c>
+      <c r="C127" t="n">
+        <v>7</v>
+      </c>
+      <c r="D127" t="n">
+        <v>6.76</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>SHALVIN P</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR033</t>
+        </is>
+      </c>
+      <c r="C128" t="n">
+        <v>7</v>
+      </c>
+      <c r="D128" t="n">
+        <v>7.33</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>SRIDHUN .P</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> GT24BCAR035</t>
+        </is>
+      </c>
+      <c r="C129" t="n">
+        <v>8</v>
+      </c>
+      <c r="D129" t="n">
         <v>8.52</v>
       </c>
     </row>

</xml_diff>